<commit_message>
pbix indicadores and new correlation ipynb
</commit_message>
<xml_diff>
--- a/DataClean/indicadores.xlsx
+++ b/DataClean/indicadores.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V77"/>
+  <dimension ref="A1:W77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,45 +501,50 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>Población activa, total</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>Población de 65 años de edad y más, hombres</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Población de 65 años de edad y más, mujeres</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Población de 65 años de edad y más, total</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Población entre 0 y 14 años de edad, hombres</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Población entre 0 y 14 años de edad, mujeres</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Población entre 0 y 14 años de edad, total</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Población entre 15 y 64 años de edad, hombres</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Población entre 15 y 64 años de edad, mujeres</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Población entre 15 y 64 años de edad, total</t>
         </is>
@@ -588,30 +593,33 @@
         <v>45.56264512070832</v>
       </c>
       <c r="N2" t="n">
+        <v>146729576</v>
+      </c>
+      <c r="O2" t="n">
         <v>14414059</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>20387123</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>34801176</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>31330276</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>29907093</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>61237370</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>93239646</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>92884214</v>
       </c>
-      <c r="V2" t="n">
+      <c r="W2" t="n">
         <v>186123865</v>
       </c>
     </row>
@@ -658,30 +666,33 @@
         <v>45.62149249726409</v>
       </c>
       <c r="N3" t="n">
+        <v>147698388</v>
+      </c>
+      <c r="O3" t="n">
         <v>14620751</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>20469861</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>35090876</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>31396354</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>29953328</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>61349552</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>94410726</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>94117935</v>
       </c>
-      <c r="V3" t="n">
+      <c r="W3" t="n">
         <v>188528528</v>
       </c>
     </row>
@@ -728,30 +739,33 @@
         <v>45.67336567392557</v>
       </c>
       <c r="N4" t="n">
+        <v>148526037</v>
+      </c>
+      <c r="O4" t="n">
         <v>14818992</v>
       </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
         <v>20534403</v>
       </c>
-      <c r="P4" t="n">
+      <c r="Q4" t="n">
         <v>35353639</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="R4" t="n">
         <v>31501156</v>
       </c>
-      <c r="R4" t="n">
+      <c r="S4" t="n">
         <v>30039941</v>
       </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
         <v>61540958</v>
       </c>
-      <c r="T4" t="n">
+      <c r="U4" t="n">
         <v>95474911</v>
       </c>
-      <c r="U4" t="n">
+      <c r="V4" t="n">
         <v>95255789</v>
       </c>
-      <c r="V4" t="n">
+      <c r="W4" t="n">
         <v>190730595</v>
       </c>
     </row>
@@ -798,30 +812,33 @@
         <v>45.82367135144958</v>
       </c>
       <c r="N5" t="n">
+        <v>149140813</v>
+      </c>
+      <c r="O5" t="n">
         <v>15016619</v>
       </c>
-      <c r="O5" t="n">
+      <c r="P5" t="n">
         <v>20601784</v>
       </c>
-      <c r="P5" t="n">
+      <c r="Q5" t="n">
         <v>35618525</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="R5" t="n">
         <v>31584885</v>
       </c>
-      <c r="R5" t="n">
+      <c r="S5" t="n">
         <v>30115848</v>
       </c>
-      <c r="S5" t="n">
+      <c r="T5" t="n">
         <v>61700652</v>
       </c>
-      <c r="T5" t="n">
+      <c r="U5" t="n">
         <v>96471064</v>
       </c>
-      <c r="U5" t="n">
+      <c r="V5" t="n">
         <v>96317733</v>
       </c>
-      <c r="V5" t="n">
+      <c r="W5" t="n">
         <v>192788756</v>
       </c>
     </row>
@@ -868,30 +885,33 @@
         <v>45.75482603800209</v>
       </c>
       <c r="N6" t="n">
+        <v>150211571</v>
+      </c>
+      <c r="O6" t="n">
         <v>15239541</v>
       </c>
-      <c r="O6" t="n">
+      <c r="P6" t="n">
         <v>20724462</v>
       </c>
-      <c r="P6" t="n">
+      <c r="Q6" t="n">
         <v>35964061</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="R6" t="n">
         <v>31622791</v>
       </c>
-      <c r="R6" t="n">
+      <c r="S6" t="n">
         <v>30158889</v>
       </c>
-      <c r="S6" t="n">
+      <c r="T6" t="n">
         <v>61781645</v>
       </c>
-      <c r="T6" t="n">
+      <c r="U6" t="n">
         <v>97587329</v>
       </c>
-      <c r="U6" t="n">
+      <c r="V6" t="n">
         <v>97472285</v>
       </c>
-      <c r="V6" t="n">
+      <c r="W6" t="n">
         <v>195059592</v>
       </c>
     </row>
@@ -938,30 +958,33 @@
         <v>45.78730687761242</v>
       </c>
       <c r="N7" t="n">
+        <v>152071960</v>
+      </c>
+      <c r="O7" t="n">
         <v>15480384</v>
       </c>
-      <c r="O7" t="n">
+      <c r="P7" t="n">
         <v>20902768</v>
       </c>
-      <c r="P7" t="n">
+      <c r="Q7" t="n">
         <v>36383151</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="R7" t="n">
         <v>31577348</v>
       </c>
-      <c r="R7" t="n">
+      <c r="S7" t="n">
         <v>30129872</v>
       </c>
-      <c r="S7" t="n">
+      <c r="T7" t="n">
         <v>61707218</v>
       </c>
-      <c r="T7" t="n">
+      <c r="U7" t="n">
         <v>98768475</v>
       </c>
-      <c r="U7" t="n">
+      <c r="V7" t="n">
         <v>98657753</v>
       </c>
-      <c r="V7" t="n">
+      <c r="W7" t="n">
         <v>197426230</v>
       </c>
     </row>
@@ -1008,30 +1031,33 @@
         <v>45.76963741468034</v>
       </c>
       <c r="N8" t="n">
+        <v>153931108</v>
+      </c>
+      <c r="O8" t="n">
         <v>15790766</v>
       </c>
-      <c r="O8" t="n">
+      <c r="P8" t="n">
         <v>21152004</v>
       </c>
-      <c r="P8" t="n">
+      <c r="Q8" t="n">
         <v>36942166</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="R8" t="n">
         <v>31782381</v>
       </c>
-      <c r="R8" t="n">
+      <c r="S8" t="n">
         <v>30332735</v>
       </c>
-      <c r="S8" t="n">
+      <c r="T8" t="n">
         <v>62115320</v>
       </c>
-      <c r="T8" t="n">
+      <c r="U8" t="n">
         <v>99695551</v>
       </c>
-      <c r="U8" t="n">
+      <c r="V8" t="n">
         <v>99626475</v>
       </c>
-      <c r="V8" t="n">
+      <c r="W8" t="n">
         <v>199322426</v>
       </c>
     </row>
@@ -1078,30 +1104,33 @@
         <v>45.82259042493703</v>
       </c>
       <c r="N9" t="n">
+        <v>155224880</v>
+      </c>
+      <c r="O9" t="n">
         <v>16118061</v>
       </c>
-      <c r="O9" t="n">
+      <c r="P9" t="n">
         <v>21452009</v>
       </c>
-      <c r="P9" t="n">
+      <c r="Q9" t="n">
         <v>37569159</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="R9" t="n">
         <v>31886002</v>
       </c>
-      <c r="R9" t="n">
+      <c r="S9" t="n">
         <v>30438116</v>
       </c>
-      <c r="S9" t="n">
+      <c r="T9" t="n">
         <v>62324459</v>
       </c>
-      <c r="T9" t="n">
+      <c r="U9" t="n">
         <v>100693346</v>
       </c>
-      <c r="U9" t="n">
+      <c r="V9" t="n">
         <v>100643672</v>
       </c>
-      <c r="V9" t="n">
+      <c r="W9" t="n">
         <v>201337589</v>
       </c>
     </row>
@@ -1148,30 +1177,33 @@
         <v>45.97300854311695</v>
       </c>
       <c r="N10" t="n">
+        <v>157006864</v>
+      </c>
+      <c r="O10" t="n">
         <v>16483342</v>
       </c>
-      <c r="O10" t="n">
+      <c r="P10" t="n">
         <v>21818559</v>
       </c>
-      <c r="P10" t="n">
+      <c r="Q10" t="n">
         <v>38300984</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="R10" t="n">
         <v>31928302</v>
       </c>
-      <c r="R10" t="n">
+      <c r="S10" t="n">
         <v>30486117</v>
       </c>
-      <c r="S10" t="n">
+      <c r="T10" t="n">
         <v>62414797</v>
       </c>
-      <c r="T10" t="n">
+      <c r="U10" t="n">
         <v>101717388</v>
       </c>
-      <c r="U10" t="n">
+      <c r="V10" t="n">
         <v>101660259</v>
       </c>
-      <c r="V10" t="n">
+      <c r="W10" t="n">
         <v>203378186</v>
       </c>
     </row>
@@ -1218,30 +1250,33 @@
         <v>46.18004002615657</v>
       </c>
       <c r="N11" t="n">
+        <v>157109264</v>
+      </c>
+      <c r="O11" t="n">
         <v>16901413</v>
       </c>
-      <c r="O11" t="n">
+      <c r="P11" t="n">
         <v>22251373</v>
       </c>
-      <c r="P11" t="n">
+      <c r="Q11" t="n">
         <v>39152172</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="R11" t="n">
         <v>31946371</v>
       </c>
-      <c r="R11" t="n">
+      <c r="S11" t="n">
         <v>30509793</v>
       </c>
-      <c r="S11" t="n">
+      <c r="T11" t="n">
         <v>62456435</v>
       </c>
-      <c r="T11" t="n">
+      <c r="U11" t="n">
         <v>102625726</v>
       </c>
-      <c r="U11" t="n">
+      <c r="V11" t="n">
         <v>102536853</v>
       </c>
-      <c r="V11" t="n">
+      <c r="W11" t="n">
         <v>205162922</v>
       </c>
     </row>
@@ -1288,30 +1323,33 @@
         <v>46.18389040235681</v>
       </c>
       <c r="N12" t="n">
+        <v>156903447</v>
+      </c>
+      <c r="O12" t="n">
         <v>17391871</v>
       </c>
-      <c r="O12" t="n">
+      <c r="P12" t="n">
         <v>22763564</v>
       </c>
-      <c r="P12" t="n">
+      <c r="Q12" t="n">
         <v>40155435</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="R12" t="n">
         <v>31967004</v>
       </c>
-      <c r="R12" t="n">
+      <c r="S12" t="n">
         <v>30530820</v>
       </c>
-      <c r="S12" t="n">
+      <c r="T12" t="n">
         <v>62497826</v>
       </c>
-      <c r="T12" t="n">
+      <c r="U12" t="n">
         <v>103405231</v>
       </c>
-      <c r="U12" t="n">
+      <c r="V12" t="n">
         <v>103263176</v>
       </c>
-      <c r="V12" t="n">
+      <c r="W12" t="n">
         <v>206668404</v>
       </c>
     </row>
@@ -1358,30 +1396,33 @@
         <v>46.1111440993089</v>
       </c>
       <c r="N13" t="n">
+        <v>156975333</v>
+      </c>
+      <c r="O13" t="n">
         <v>17962743</v>
       </c>
-      <c r="O13" t="n">
+      <c r="P13" t="n">
         <v>23320072</v>
       </c>
-      <c r="P13" t="n">
+      <c r="Q13" t="n">
         <v>41282103</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="R13" t="n">
         <v>31898118</v>
       </c>
-      <c r="R13" t="n">
+      <c r="S13" t="n">
         <v>30491299</v>
       </c>
-      <c r="S13" t="n">
+      <c r="T13" t="n">
         <v>62389679</v>
       </c>
-      <c r="T13" t="n">
+      <c r="U13" t="n">
         <v>104049469</v>
       </c>
-      <c r="U13" t="n">
+      <c r="V13" t="n">
         <v>103835172</v>
       </c>
-      <c r="V13" t="n">
+      <c r="W13" t="n">
         <v>207885093</v>
       </c>
     </row>
@@ -1428,30 +1469,33 @@
         <v>45.93917299473114</v>
       </c>
       <c r="N14" t="n">
+        <v>158636184</v>
+      </c>
+      <c r="O14" t="n">
         <v>18603482</v>
       </c>
-      <c r="O14" t="n">
+      <c r="P14" t="n">
         <v>23957268</v>
       </c>
-      <c r="P14" t="n">
+      <c r="Q14" t="n">
         <v>42559976</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="R14" t="n">
         <v>31801547</v>
       </c>
-      <c r="R14" t="n">
+      <c r="S14" t="n">
         <v>30409425</v>
       </c>
-      <c r="S14" t="n">
+      <c r="T14" t="n">
         <v>62211250</v>
       </c>
-      <c r="T14" t="n">
+      <c r="U14" t="n">
         <v>104679561</v>
       </c>
-      <c r="U14" t="n">
+      <c r="V14" t="n">
         <v>104379707</v>
       </c>
-      <c r="V14" t="n">
+      <c r="W14" t="n">
         <v>209059763</v>
       </c>
     </row>
@@ -1498,30 +1542,33 @@
         <v>45.91003624373574</v>
       </c>
       <c r="N15" t="n">
+        <v>158755710</v>
+      </c>
+      <c r="O15" t="n">
         <v>19289958</v>
       </c>
-      <c r="O15" t="n">
+      <c r="P15" t="n">
         <v>24649583</v>
       </c>
-      <c r="P15" t="n">
+      <c r="Q15" t="n">
         <v>43939066</v>
       </c>
-      <c r="Q15" t="n">
+      <c r="R15" t="n">
         <v>31687668</v>
       </c>
-      <c r="R15" t="n">
+      <c r="S15" t="n">
         <v>30300803</v>
       </c>
-      <c r="S15" t="n">
+      <c r="T15" t="n">
         <v>61988641</v>
       </c>
-      <c r="T15" t="n">
+      <c r="U15" t="n">
         <v>105229771</v>
       </c>
-      <c r="U15" t="n">
+      <c r="V15" t="n">
         <v>104835932</v>
       </c>
-      <c r="V15" t="n">
+      <c r="W15" t="n">
         <v>210066008</v>
       </c>
     </row>
@@ -1568,30 +1615,33 @@
         <v>45.96584791839523</v>
       </c>
       <c r="N16" t="n">
+        <v>159532062</v>
+      </c>
+      <c r="O16" t="n">
         <v>20015668</v>
       </c>
-      <c r="O16" t="n">
+      <c r="P16" t="n">
         <v>25398693</v>
       </c>
-      <c r="P16" t="n">
+      <c r="Q16" t="n">
         <v>45414232</v>
       </c>
-      <c r="Q16" t="n">
+      <c r="R16" t="n">
         <v>31593585</v>
       </c>
-      <c r="R16" t="n">
+      <c r="S16" t="n">
         <v>30208459</v>
       </c>
-      <c r="S16" t="n">
+      <c r="T16" t="n">
         <v>61802095</v>
       </c>
-      <c r="T16" t="n">
+      <c r="U16" t="n">
         <v>105788452</v>
       </c>
-      <c r="U16" t="n">
+      <c r="V16" t="n">
         <v>105296151</v>
       </c>
-      <c r="V16" t="n">
+      <c r="W16" t="n">
         <v>211084681</v>
       </c>
     </row>
@@ -1638,30 +1688,33 @@
         <v>45.86337744628997</v>
       </c>
       <c r="N17" t="n">
+        <v>160596354</v>
+      </c>
+      <c r="O17" t="n">
         <v>20761867</v>
       </c>
-      <c r="O17" t="n">
+      <c r="P17" t="n">
         <v>26188371</v>
       </c>
-      <c r="P17" t="n">
+      <c r="Q17" t="n">
         <v>46950237</v>
       </c>
-      <c r="Q17" t="n">
+      <c r="R17" t="n">
         <v>31510030</v>
       </c>
-      <c r="R17" t="n">
+      <c r="S17" t="n">
         <v>30127998</v>
       </c>
-      <c r="S17" t="n">
+      <c r="T17" t="n">
         <v>61638027</v>
       </c>
-      <c r="T17" t="n">
+      <c r="U17" t="n">
         <v>106319959</v>
       </c>
-      <c r="U17" t="n">
+      <c r="V17" t="n">
         <v>105726939</v>
       </c>
-      <c r="V17" t="n">
+      <c r="W17" t="n">
         <v>212046899</v>
       </c>
     </row>
@@ -1708,30 +1761,33 @@
         <v>45.87067996395123</v>
       </c>
       <c r="N18" t="n">
+        <v>162547573</v>
+      </c>
+      <c r="O18" t="n">
         <v>21550046</v>
       </c>
-      <c r="O18" t="n">
+      <c r="P18" t="n">
         <v>26999911</v>
       </c>
-      <c r="P18" t="n">
+      <c r="Q18" t="n">
         <v>48549959</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="R18" t="n">
         <v>31404869</v>
       </c>
-      <c r="R18" t="n">
+      <c r="S18" t="n">
         <v>30029421</v>
       </c>
-      <c r="S18" t="n">
+      <c r="T18" t="n">
         <v>61434232</v>
       </c>
-      <c r="T18" t="n">
+      <c r="U18" t="n">
         <v>106806372</v>
       </c>
-      <c r="U18" t="n">
+      <c r="V18" t="n">
         <v>106150693</v>
       </c>
-      <c r="V18" t="n">
+      <c r="W18" t="n">
         <v>212957120</v>
       </c>
     </row>
@@ -1778,30 +1834,33 @@
         <v>46.02508330606134</v>
       </c>
       <c r="N19" t="n">
+        <v>164268059</v>
+      </c>
+      <c r="O19" t="n">
         <v>22314476</v>
       </c>
-      <c r="O19" t="n">
+      <c r="P19" t="n">
         <v>27796212</v>
       </c>
-      <c r="P19" t="n">
+      <c r="Q19" t="n">
         <v>50110709</v>
       </c>
-      <c r="Q19" t="n">
+      <c r="R19" t="n">
         <v>31327678</v>
       </c>
-      <c r="R19" t="n">
+      <c r="S19" t="n">
         <v>29959876</v>
       </c>
-      <c r="S19" t="n">
+      <c r="T19" t="n">
         <v>61287489</v>
       </c>
-      <c r="T19" t="n">
+      <c r="U19" t="n">
         <v>107149699</v>
       </c>
-      <c r="U19" t="n">
+      <c r="V19" t="n">
         <v>106437598</v>
       </c>
-      <c r="V19" t="n">
+      <c r="W19" t="n">
         <v>213587340</v>
       </c>
     </row>
@@ -1848,30 +1907,33 @@
         <v>46.05367449881579</v>
       </c>
       <c r="N20" t="n">
+        <v>165483017</v>
+      </c>
+      <c r="O20" t="n">
         <v>23058935</v>
       </c>
-      <c r="O20" t="n">
+      <c r="P20" t="n">
         <v>28582660</v>
       </c>
-      <c r="P20" t="n">
+      <c r="Q20" t="n">
         <v>51641630</v>
       </c>
-      <c r="Q20" t="n">
+      <c r="R20" t="n">
         <v>31239420</v>
       </c>
-      <c r="R20" t="n">
+      <c r="S20" t="n">
         <v>29880716</v>
       </c>
-      <c r="S20" t="n">
+      <c r="T20" t="n">
         <v>61120095</v>
       </c>
-      <c r="T20" t="n">
+      <c r="U20" t="n">
         <v>107346573</v>
       </c>
-      <c r="U20" t="n">
+      <c r="V20" t="n">
         <v>106579196</v>
       </c>
-      <c r="V20" t="n">
+      <c r="W20" t="n">
         <v>213925776</v>
       </c>
     </row>
@@ -1918,30 +1980,33 @@
         <v>40.35360001889646</v>
       </c>
       <c r="N21" t="n">
+        <v>67652881</v>
+      </c>
+      <c r="O21" t="n">
         <v>8956200</v>
       </c>
-      <c r="O21" t="n">
+      <c r="P21" t="n">
         <v>12587381</v>
       </c>
-      <c r="P21" t="n">
+      <c r="Q21" t="n">
         <v>21543580</v>
       </c>
-      <c r="Q21" t="n">
+      <c r="R21" t="n">
         <v>9625977</v>
       </c>
-      <c r="R21" t="n">
+      <c r="S21" t="n">
         <v>9126335</v>
       </c>
-      <c r="S21" t="n">
+      <c r="T21" t="n">
         <v>18752313</v>
       </c>
-      <c r="T21" t="n">
+      <c r="U21" t="n">
         <v>43707887</v>
       </c>
-      <c r="U21" t="n">
+      <c r="V21" t="n">
         <v>42839220</v>
       </c>
-      <c r="V21" t="n">
+      <c r="W21" t="n">
         <v>86547107</v>
       </c>
     </row>
@@ -1988,30 +2053,33 @@
         <v>40.55620078744671</v>
       </c>
       <c r="N22" t="n">
+        <v>67601019</v>
+      </c>
+      <c r="O22" t="n">
         <v>9282301</v>
       </c>
-      <c r="O22" t="n">
+      <c r="P22" t="n">
         <v>12978169</v>
       </c>
-      <c r="P22" t="n">
+      <c r="Q22" t="n">
         <v>22260296</v>
       </c>
-      <c r="Q22" t="n">
+      <c r="R22" t="n">
         <v>9515389</v>
       </c>
-      <c r="R22" t="n">
+      <c r="S22" t="n">
         <v>9021855</v>
       </c>
-      <c r="S22" t="n">
+      <c r="T22" t="n">
         <v>18537284</v>
       </c>
-      <c r="T22" t="n">
+      <c r="U22" t="n">
         <v>43615246</v>
       </c>
-      <c r="U22" t="n">
+      <c r="V22" t="n">
         <v>42736040</v>
       </c>
-      <c r="V22" t="n">
+      <c r="W22" t="n">
         <v>86351420</v>
       </c>
     </row>
@@ -2058,30 +2126,33 @@
         <v>40.5240480316177</v>
       </c>
       <c r="N23" t="n">
+        <v>67173003</v>
+      </c>
+      <c r="O23" t="n">
         <v>9608821</v>
       </c>
-      <c r="O23" t="n">
+      <c r="P23" t="n">
         <v>13370380</v>
       </c>
-      <c r="P23" t="n">
+      <c r="Q23" t="n">
         <v>22978947</v>
       </c>
-      <c r="Q23" t="n">
+      <c r="R23" t="n">
         <v>9398422</v>
       </c>
-      <c r="R23" t="n">
+      <c r="S23" t="n">
         <v>8910849</v>
       </c>
-      <c r="S23" t="n">
+      <c r="T23" t="n">
         <v>18309332</v>
       </c>
-      <c r="T23" t="n">
+      <c r="U23" t="n">
         <v>43524231</v>
       </c>
-      <c r="U23" t="n">
+      <c r="V23" t="n">
         <v>42632297</v>
       </c>
-      <c r="V23" t="n">
+      <c r="W23" t="n">
         <v>86156721</v>
       </c>
     </row>
@@ -2128,30 +2199,33 @@
         <v>40.69544212825535</v>
       </c>
       <c r="N24" t="n">
+        <v>67065336</v>
+      </c>
+      <c r="O24" t="n">
         <v>9936892</v>
       </c>
-      <c r="O24" t="n">
+      <c r="P24" t="n">
         <v>13766451</v>
       </c>
-      <c r="P24" t="n">
+      <c r="Q24" t="n">
         <v>23703098</v>
       </c>
-      <c r="Q24" t="n">
+      <c r="R24" t="n">
         <v>9283012</v>
       </c>
-      <c r="R24" t="n">
+      <c r="S24" t="n">
         <v>8800893</v>
       </c>
-      <c r="S24" t="n">
+      <c r="T24" t="n">
         <v>18083961</v>
       </c>
-      <c r="T24" t="n">
+      <c r="U24" t="n">
         <v>43419292</v>
       </c>
-      <c r="U24" t="n">
+      <c r="V24" t="n">
         <v>42511460</v>
       </c>
-      <c r="V24" t="n">
+      <c r="W24" t="n">
         <v>85930942</v>
       </c>
     </row>
@@ -2198,30 +2272,33 @@
         <v>40.85281230164463</v>
       </c>
       <c r="N25" t="n">
+        <v>66725257</v>
+      </c>
+      <c r="O25" t="n">
         <v>10251173</v>
       </c>
-      <c r="O25" t="n">
+      <c r="P25" t="n">
         <v>14148188</v>
       </c>
-      <c r="P25" t="n">
+      <c r="Q25" t="n">
         <v>24399197</v>
       </c>
-      <c r="Q25" t="n">
+      <c r="R25" t="n">
         <v>9167575</v>
       </c>
-      <c r="R25" t="n">
+      <c r="S25" t="n">
         <v>8690637</v>
       </c>
-      <c r="S25" t="n">
+      <c r="T25" t="n">
         <v>17858252</v>
       </c>
-      <c r="T25" t="n">
+      <c r="U25" t="n">
         <v>43215631</v>
       </c>
-      <c r="U25" t="n">
+      <c r="V25" t="n">
         <v>42287796</v>
       </c>
-      <c r="V25" t="n">
+      <c r="W25" t="n">
         <v>85503551</v>
       </c>
     </row>
@@ -2268,30 +2345,33 @@
         <v>40.99796817251149</v>
       </c>
       <c r="N26" t="n">
+        <v>66734012</v>
+      </c>
+      <c r="O26" t="n">
         <v>10568710</v>
       </c>
-      <c r="O26" t="n">
+      <c r="P26" t="n">
         <v>14541693</v>
       </c>
-      <c r="P26" t="n">
+      <c r="Q26" t="n">
         <v>25110400</v>
       </c>
-      <c r="Q26" t="n">
+      <c r="R26" t="n">
         <v>9072012</v>
       </c>
-      <c r="R26" t="n">
+      <c r="S26" t="n">
         <v>8598839</v>
       </c>
-      <c r="S26" t="n">
+      <c r="T26" t="n">
         <v>17670854</v>
       </c>
-      <c r="T26" t="n">
+      <c r="U26" t="n">
         <v>42973812</v>
       </c>
-      <c r="U26" t="n">
+      <c r="V26" t="n">
         <v>42017934</v>
       </c>
-      <c r="V26" t="n">
+      <c r="W26" t="n">
         <v>84991747</v>
       </c>
     </row>
@@ -2338,30 +2418,33 @@
         <v>41.12442164581217</v>
       </c>
       <c r="N27" t="n">
+        <v>66802058</v>
+      </c>
+      <c r="O27" t="n">
         <v>10885517</v>
       </c>
-      <c r="O27" t="n">
+      <c r="P27" t="n">
         <v>14912658</v>
       </c>
-      <c r="P27" t="n">
+      <c r="Q27" t="n">
         <v>25797976</v>
       </c>
-      <c r="Q27" t="n">
+      <c r="R27" t="n">
         <v>8983847</v>
       </c>
-      <c r="R27" t="n">
+      <c r="S27" t="n">
         <v>8515507</v>
       </c>
-      <c r="S27" t="n">
+      <c r="T27" t="n">
         <v>17499393</v>
       </c>
-      <c r="T27" t="n">
+      <c r="U27" t="n">
         <v>42759264</v>
       </c>
-      <c r="U27" t="n">
+      <c r="V27" t="n">
         <v>41797207</v>
       </c>
-      <c r="V27" t="n">
+      <c r="W27" t="n">
         <v>84556631</v>
       </c>
     </row>
@@ -2408,30 +2491,33 @@
         <v>41.11939552721955</v>
       </c>
       <c r="N28" t="n">
+        <v>67143470</v>
+      </c>
+      <c r="O28" t="n">
         <v>11201906</v>
       </c>
-      <c r="O28" t="n">
+      <c r="P28" t="n">
         <v>15291655</v>
       </c>
-      <c r="P28" t="n">
+      <c r="Q28" t="n">
         <v>26493151</v>
       </c>
-      <c r="Q28" t="n">
+      <c r="R28" t="n">
         <v>8928017</v>
       </c>
-      <c r="R28" t="n">
+      <c r="S28" t="n">
         <v>8463087</v>
       </c>
-      <c r="S28" t="n">
+      <c r="T28" t="n">
         <v>17391195</v>
       </c>
-      <c r="T28" t="n">
+      <c r="U28" t="n">
         <v>42545551</v>
       </c>
-      <c r="U28" t="n">
+      <c r="V28" t="n">
         <v>41570784</v>
       </c>
-      <c r="V28" t="n">
+      <c r="W28" t="n">
         <v>84116655</v>
       </c>
     </row>
@@ -2478,30 +2564,33 @@
         <v>41.25954929059262</v>
       </c>
       <c r="N29" t="n">
+        <v>67100796</v>
+      </c>
+      <c r="O29" t="n">
         <v>11520347</v>
       </c>
-      <c r="O29" t="n">
+      <c r="P29" t="n">
         <v>15675525</v>
       </c>
-      <c r="P29" t="n">
+      <c r="Q29" t="n">
         <v>27195327</v>
       </c>
-      <c r="Q29" t="n">
+      <c r="R29" t="n">
         <v>8883347</v>
       </c>
-      <c r="R29" t="n">
+      <c r="S29" t="n">
         <v>8421074</v>
       </c>
-      <c r="S29" t="n">
+      <c r="T29" t="n">
         <v>17304542</v>
       </c>
-      <c r="T29" t="n">
+      <c r="U29" t="n">
         <v>42278072</v>
       </c>
-      <c r="U29" t="n">
+      <c r="V29" t="n">
         <v>41284635</v>
       </c>
-      <c r="V29" t="n">
+      <c r="W29" t="n">
         <v>83563130</v>
       </c>
     </row>
@@ -2548,30 +2637,33 @@
         <v>41.5918159295201</v>
       </c>
       <c r="N30" t="n">
+        <v>66914282</v>
+      </c>
+      <c r="O30" t="n">
         <v>11864448</v>
       </c>
-      <c r="O30" t="n">
+      <c r="P30" t="n">
         <v>16087526</v>
       </c>
-      <c r="P30" t="n">
+      <c r="Q30" t="n">
         <v>27951519</v>
       </c>
-      <c r="Q30" t="n">
+      <c r="R30" t="n">
         <v>8834377</v>
       </c>
-      <c r="R30" t="n">
+      <c r="S30" t="n">
         <v>8374067</v>
       </c>
-      <c r="S30" t="n">
+      <c r="T30" t="n">
         <v>17208544</v>
       </c>
-      <c r="T30" t="n">
+      <c r="U30" t="n">
         <v>41952994</v>
       </c>
-      <c r="U30" t="n">
+      <c r="V30" t="n">
         <v>40933588</v>
       </c>
-      <c r="V30" t="n">
+      <c r="W30" t="n">
         <v>82886937</v>
       </c>
     </row>
@@ -2618,30 +2710,33 @@
         <v>41.73433824243273</v>
       </c>
       <c r="N31" t="n">
+        <v>66663144</v>
+      </c>
+      <c r="O31" t="n">
         <v>12257292</v>
       </c>
-      <c r="O31" t="n">
+      <c r="P31" t="n">
         <v>16555986</v>
       </c>
-      <c r="P31" t="n">
+      <c r="Q31" t="n">
         <v>28813280</v>
       </c>
-      <c r="Q31" t="n">
+      <c r="R31" t="n">
         <v>8781659</v>
       </c>
-      <c r="R31" t="n">
+      <c r="S31" t="n">
         <v>8321810</v>
       </c>
-      <c r="S31" t="n">
+      <c r="T31" t="n">
         <v>17103469</v>
       </c>
-      <c r="T31" t="n">
+      <c r="U31" t="n">
         <v>41604516</v>
       </c>
-      <c r="U31" t="n">
+      <c r="V31" t="n">
         <v>40548737</v>
       </c>
-      <c r="V31" t="n">
+      <c r="W31" t="n">
         <v>82153251</v>
       </c>
     </row>
@@ -2688,30 +2783,33 @@
         <v>41.76523217006991</v>
       </c>
       <c r="N32" t="n">
+        <v>66043052</v>
+      </c>
+      <c r="O32" t="n">
         <v>12640688</v>
       </c>
-      <c r="O32" t="n">
+      <c r="P32" t="n">
         <v>16963837</v>
       </c>
-      <c r="P32" t="n">
+      <c r="Q32" t="n">
         <v>29603888</v>
       </c>
-      <c r="Q32" t="n">
+      <c r="R32" t="n">
         <v>8732166</v>
       </c>
-      <c r="R32" t="n">
+      <c r="S32" t="n">
         <v>8277190</v>
       </c>
-      <c r="S32" t="n">
+      <c r="T32" t="n">
         <v>17009491</v>
       </c>
-      <c r="T32" t="n">
+      <c r="U32" t="n">
         <v>41137820</v>
       </c>
-      <c r="U32" t="n">
+      <c r="V32" t="n">
         <v>40081298</v>
       </c>
-      <c r="V32" t="n">
+      <c r="W32" t="n">
         <v>81219621</v>
       </c>
     </row>
@@ -2758,30 +2856,33 @@
         <v>41.93683008231884</v>
       </c>
       <c r="N33" t="n">
+        <v>65639408</v>
+      </c>
+      <c r="O33" t="n">
         <v>13061619</v>
       </c>
-      <c r="O33" t="n">
+      <c r="P33" t="n">
         <v>17414552</v>
       </c>
-      <c r="P33" t="n">
+      <c r="Q33" t="n">
         <v>30475171</v>
       </c>
-      <c r="Q33" t="n">
+      <c r="R33" t="n">
         <v>8675816</v>
       </c>
-      <c r="R33" t="n">
+      <c r="S33" t="n">
         <v>8225217</v>
       </c>
-      <c r="S33" t="n">
+      <c r="T33" t="n">
         <v>16901251</v>
       </c>
-      <c r="T33" t="n">
+      <c r="U33" t="n">
         <v>40659104</v>
       </c>
-      <c r="U33" t="n">
+      <c r="V33" t="n">
         <v>39592692</v>
       </c>
-      <c r="V33" t="n">
+      <c r="W33" t="n">
         <v>80252578</v>
       </c>
     </row>
@@ -2828,30 +2929,33 @@
         <v>42.34860616044202</v>
       </c>
       <c r="N34" t="n">
+        <v>65970039</v>
+      </c>
+      <c r="O34" t="n">
         <v>13497300</v>
       </c>
-      <c r="O34" t="n">
+      <c r="P34" t="n">
         <v>17887816</v>
       </c>
-      <c r="P34" t="n">
+      <c r="Q34" t="n">
         <v>31384095</v>
       </c>
-      <c r="Q34" t="n">
+      <c r="R34" t="n">
         <v>8613124</v>
       </c>
-      <c r="R34" t="n">
+      <c r="S34" t="n">
         <v>8165949</v>
       </c>
-      <c r="S34" t="n">
+      <c r="T34" t="n">
         <v>16779297</v>
       </c>
-      <c r="T34" t="n">
+      <c r="U34" t="n">
         <v>40183780</v>
       </c>
-      <c r="U34" t="n">
+      <c r="V34" t="n">
         <v>39097031</v>
       </c>
-      <c r="V34" t="n">
+      <c r="W34" t="n">
         <v>79281609</v>
       </c>
     </row>
@@ -2898,30 +3002,33 @@
         <v>42.59072794138059</v>
       </c>
       <c r="N35" t="n">
+        <v>66175617</v>
+      </c>
+      <c r="O35" t="n">
         <v>13914095</v>
       </c>
-      <c r="O35" t="n">
+      <c r="P35" t="n">
         <v>18350685</v>
       </c>
-      <c r="P35" t="n">
+      <c r="Q35" t="n">
         <v>32264097</v>
       </c>
-      <c r="Q35" t="n">
+      <c r="R35" t="n">
         <v>8547248</v>
       </c>
-      <c r="R35" t="n">
+      <c r="S35" t="n">
         <v>8102183</v>
       </c>
-      <c r="S35" t="n">
+      <c r="T35" t="n">
         <v>16649583</v>
       </c>
-      <c r="T35" t="n">
+      <c r="U35" t="n">
         <v>39739205</v>
       </c>
-      <c r="U35" t="n">
+      <c r="V35" t="n">
         <v>38622584</v>
       </c>
-      <c r="V35" t="n">
+      <c r="W35" t="n">
         <v>78362321</v>
       </c>
     </row>
@@ -2968,30 +3075,33 @@
         <v>42.80516572882726</v>
       </c>
       <c r="N36" t="n">
+        <v>66363530</v>
+      </c>
+      <c r="O36" t="n">
         <v>14294734</v>
       </c>
-      <c r="O36" t="n">
+      <c r="P36" t="n">
         <v>18786503</v>
       </c>
-      <c r="P36" t="n">
+      <c r="Q36" t="n">
         <v>33081239</v>
       </c>
-      <c r="Q36" t="n">
+      <c r="R36" t="n">
         <v>8479674</v>
       </c>
-      <c r="R36" t="n">
+      <c r="S36" t="n">
         <v>8035159</v>
       </c>
-      <c r="S36" t="n">
+      <c r="T36" t="n">
         <v>16514831</v>
       </c>
-      <c r="T36" t="n">
+      <c r="U36" t="n">
         <v>39349870</v>
       </c>
-      <c r="U36" t="n">
+      <c r="V36" t="n">
         <v>38195060</v>
       </c>
-      <c r="V36" t="n">
+      <c r="W36" t="n">
         <v>77544929</v>
       </c>
     </row>
@@ -3038,30 +3148,33 @@
         <v>43.11094792170073</v>
       </c>
       <c r="N37" t="n">
+        <v>66850743</v>
+      </c>
+      <c r="O37" t="n">
         <v>14634284</v>
       </c>
-      <c r="O37" t="n">
+      <c r="P37" t="n">
         <v>19136532</v>
       </c>
-      <c r="P37" t="n">
+      <c r="Q37" t="n">
         <v>33770147</v>
       </c>
-      <c r="Q37" t="n">
+      <c r="R37" t="n">
         <v>8420062</v>
       </c>
-      <c r="R37" t="n">
+      <c r="S37" t="n">
         <v>7980334</v>
       </c>
-      <c r="S37" t="n">
+      <c r="T37" t="n">
         <v>16400528</v>
       </c>
-      <c r="T37" t="n">
+      <c r="U37" t="n">
         <v>38988697</v>
       </c>
-      <c r="U37" t="n">
+      <c r="V37" t="n">
         <v>37834602</v>
       </c>
-      <c r="V37" t="n">
+      <c r="W37" t="n">
         <v>76823835</v>
       </c>
     </row>
@@ -3108,30 +3221,33 @@
         <v>43.50272145024488</v>
       </c>
       <c r="N38" t="n">
+        <v>67288388</v>
+      </c>
+      <c r="O38" t="n">
         <v>14930064</v>
       </c>
-      <c r="O38" t="n">
+      <c r="P38" t="n">
         <v>19441927</v>
       </c>
-      <c r="P38" t="n">
+      <c r="Q38" t="n">
         <v>34370970</v>
       </c>
-      <c r="Q38" t="n">
+      <c r="R38" t="n">
         <v>8340585</v>
       </c>
-      <c r="R38" t="n">
+      <c r="S38" t="n">
         <v>7906038</v>
       </c>
-      <c r="S38" t="n">
+      <c r="T38" t="n">
         <v>16246827</v>
       </c>
-      <c r="T38" t="n">
+      <c r="U38" t="n">
         <v>38661365</v>
       </c>
-      <c r="U38" t="n">
+      <c r="V38" t="n">
         <v>37505818</v>
       </c>
-      <c r="V38" t="n">
+      <c r="W38" t="n">
         <v>76168000</v>
       </c>
     </row>
@@ -3178,30 +3294,33 @@
         <v>43.93586330393776</v>
       </c>
       <c r="N39" t="n">
+        <v>68358370</v>
+      </c>
+      <c r="O39" t="n">
         <v>15185127</v>
       </c>
-      <c r="O39" t="n">
+      <c r="P39" t="n">
         <v>19708026</v>
       </c>
-      <c r="P39" t="n">
+      <c r="Q39" t="n">
         <v>34892133</v>
       </c>
-      <c r="Q39" t="n">
+      <c r="R39" t="n">
         <v>8247185</v>
       </c>
-      <c r="R39" t="n">
+      <c r="S39" t="n">
         <v>7817817</v>
       </c>
-      <c r="S39" t="n">
+      <c r="T39" t="n">
         <v>16065209</v>
       </c>
-      <c r="T39" t="n">
+      <c r="U39" t="n">
         <v>38365439</v>
       </c>
-      <c r="U39" t="n">
+      <c r="V39" t="n">
         <v>37205507</v>
       </c>
-      <c r="V39" t="n">
+      <c r="W39" t="n">
         <v>75571759</v>
       </c>
     </row>
@@ -3248,30 +3367,33 @@
         <v>39.4934768056119</v>
       </c>
       <c r="N40" t="n">
+        <v>2760410612</v>
+      </c>
+      <c r="O40" t="n">
         <v>182952454</v>
       </c>
-      <c r="O40" t="n">
+      <c r="P40" t="n">
         <v>237176353</v>
       </c>
-      <c r="P40" t="n">
+      <c r="Q40" t="n">
         <v>420128869</v>
       </c>
-      <c r="Q40" t="n">
+      <c r="R40" t="n">
         <v>949936770</v>
       </c>
-      <c r="R40" t="n">
+      <c r="S40" t="n">
         <v>893280463</v>
       </c>
-      <c r="S40" t="n">
+      <c r="T40" t="n">
         <v>1843217225</v>
       </c>
-      <c r="T40" t="n">
+      <c r="U40" t="n">
         <v>1944338062</v>
       </c>
-      <c r="U40" t="n">
+      <c r="V40" t="n">
         <v>1904116650</v>
       </c>
-      <c r="V40" t="n">
+      <c r="W40" t="n">
         <v>3848454670</v>
       </c>
     </row>
@@ -3318,30 +3440,33 @@
         <v>39.47470861656299</v>
       </c>
       <c r="N41" t="n">
+        <v>2797040580</v>
+      </c>
+      <c r="O41" t="n">
         <v>188218654</v>
       </c>
-      <c r="O41" t="n">
+      <c r="P41" t="n">
         <v>242573155</v>
       </c>
-      <c r="P41" t="n">
+      <c r="Q41" t="n">
         <v>430789741</v>
       </c>
-      <c r="Q41" t="n">
+      <c r="R41" t="n">
         <v>951979507</v>
       </c>
-      <c r="R41" t="n">
+      <c r="S41" t="n">
         <v>894521217</v>
       </c>
-      <c r="S41" t="n">
+      <c r="T41" t="n">
         <v>1846494859</v>
       </c>
-      <c r="T41" t="n">
+      <c r="U41" t="n">
         <v>1977317436</v>
       </c>
-      <c r="U41" t="n">
+      <c r="V41" t="n">
         <v>1936530565</v>
       </c>
-      <c r="V41" t="n">
+      <c r="W41" t="n">
         <v>3913855934</v>
       </c>
     </row>
@@ -3388,30 +3513,33 @@
         <v>39.47569687024211</v>
       </c>
       <c r="N42" t="n">
+        <v>2838912969</v>
+      </c>
+      <c r="O42" t="n">
         <v>193541290</v>
       </c>
-      <c r="O42" t="n">
+      <c r="P42" t="n">
         <v>248226002</v>
       </c>
-      <c r="P42" t="n">
+      <c r="Q42" t="n">
         <v>441763952</v>
       </c>
-      <c r="Q42" t="n">
+      <c r="R42" t="n">
         <v>951337841</v>
       </c>
-      <c r="R42" t="n">
+      <c r="S42" t="n">
         <v>892966461</v>
       </c>
-      <c r="S42" t="n">
+      <c r="T42" t="n">
         <v>1844294891</v>
       </c>
-      <c r="T42" t="n">
+      <c r="U42" t="n">
         <v>2012898903</v>
       </c>
-      <c r="U42" t="n">
+      <c r="V42" t="n">
         <v>1971223387</v>
       </c>
-      <c r="V42" t="n">
+      <c r="W42" t="n">
         <v>3984135046</v>
       </c>
     </row>
@@ -3458,30 +3586,33 @@
         <v>39.50919926773386</v>
       </c>
       <c r="N43" t="n">
+        <v>2883821977</v>
+      </c>
+      <c r="O43" t="n">
         <v>198763477</v>
       </c>
-      <c r="O43" t="n">
+      <c r="P43" t="n">
         <v>253971693</v>
       </c>
-      <c r="P43" t="n">
+      <c r="Q43" t="n">
         <v>452731716</v>
       </c>
-      <c r="Q43" t="n">
+      <c r="R43" t="n">
         <v>949166238</v>
       </c>
-      <c r="R43" t="n">
+      <c r="S43" t="n">
         <v>889858375</v>
       </c>
-      <c r="S43" t="n">
+      <c r="T43" t="n">
         <v>1839014803</v>
       </c>
-      <c r="T43" t="n">
+      <c r="U43" t="n">
         <v>2050233932</v>
       </c>
-      <c r="U43" t="n">
+      <c r="V43" t="n">
         <v>2007338808</v>
       </c>
-      <c r="V43" t="n">
+      <c r="W43" t="n">
         <v>4057586010</v>
       </c>
     </row>
@@ -3528,30 +3659,33 @@
         <v>39.48706096916199</v>
       </c>
       <c r="N44" t="n">
+        <v>2932247001</v>
+      </c>
+      <c r="O44" t="n">
         <v>203579405</v>
       </c>
-      <c r="O44" t="n">
+      <c r="P44" t="n">
         <v>259457917</v>
       </c>
-      <c r="P44" t="n">
+      <c r="Q44" t="n">
         <v>463035050</v>
       </c>
-      <c r="Q44" t="n">
+      <c r="R44" t="n">
         <v>947539333</v>
       </c>
-      <c r="R44" t="n">
+      <c r="S44" t="n">
         <v>887364917</v>
       </c>
-      <c r="S44" t="n">
+      <c r="T44" t="n">
         <v>1834897738</v>
       </c>
-      <c r="T44" t="n">
+      <c r="U44" t="n">
         <v>2087738618</v>
       </c>
-      <c r="U44" t="n">
+      <c r="V44" t="n">
         <v>2043337178</v>
       </c>
-      <c r="V44" t="n">
+      <c r="W44" t="n">
         <v>4131084573</v>
       </c>
     </row>
@@ -3598,30 +3732,33 @@
         <v>39.50303701810243</v>
       </c>
       <c r="N45" t="n">
+        <v>2978118240</v>
+      </c>
+      <c r="O45" t="n">
         <v>207872757</v>
       </c>
-      <c r="O45" t="n">
+      <c r="P45" t="n">
         <v>264534249</v>
       </c>
-      <c r="P45" t="n">
+      <c r="Q45" t="n">
         <v>472407100</v>
       </c>
-      <c r="Q45" t="n">
+      <c r="R45" t="n">
         <v>947552199</v>
       </c>
-      <c r="R45" t="n">
+      <c r="S45" t="n">
         <v>886624808</v>
       </c>
-      <c r="S45" t="n">
+      <c r="T45" t="n">
         <v>1834176990</v>
       </c>
-      <c r="T45" t="n">
+      <c r="U45" t="n">
         <v>2124394076</v>
       </c>
-      <c r="U45" t="n">
+      <c r="V45" t="n">
         <v>2078256581</v>
       </c>
-      <c r="V45" t="n">
+      <c r="W45" t="n">
         <v>4202650595</v>
       </c>
     </row>
@@ -3668,30 +3805,33 @@
         <v>39.41439569865855</v>
       </c>
       <c r="N46" t="n">
+        <v>3014743223</v>
+      </c>
+      <c r="O46" t="n">
         <v>212957354</v>
       </c>
-      <c r="O46" t="n">
+      <c r="P46" t="n">
         <v>269942107</v>
       </c>
-      <c r="P46" t="n">
+      <c r="Q46" t="n">
         <v>482896162</v>
       </c>
-      <c r="Q46" t="n">
+      <c r="R46" t="n">
         <v>949437926</v>
       </c>
-      <c r="R46" t="n">
+      <c r="S46" t="n">
         <v>887674407</v>
       </c>
-      <c r="S46" t="n">
+      <c r="T46" t="n">
         <v>1837112292</v>
       </c>
-      <c r="T46" t="n">
+      <c r="U46" t="n">
         <v>2158768472</v>
       </c>
-      <c r="U46" t="n">
+      <c r="V46" t="n">
         <v>2111453512</v>
       </c>
-      <c r="V46" t="n">
+      <c r="W46" t="n">
         <v>4270225325</v>
       </c>
     </row>
@@ -3738,30 +3878,33 @@
         <v>39.37236370068285</v>
       </c>
       <c r="N47" t="n">
+        <v>3054910370</v>
+      </c>
+      <c r="O47" t="n">
         <v>217597595</v>
       </c>
-      <c r="O47" t="n">
+      <c r="P47" t="n">
         <v>274996267</v>
       </c>
-      <c r="P47" t="n">
+      <c r="Q47" t="n">
         <v>492589391</v>
       </c>
-      <c r="Q47" t="n">
+      <c r="R47" t="n">
         <v>952666280</v>
       </c>
-      <c r="R47" t="n">
+      <c r="S47" t="n">
         <v>890214897</v>
       </c>
-      <c r="S47" t="n">
+      <c r="T47" t="n">
         <v>1842883827</v>
       </c>
-      <c r="T47" t="n">
+      <c r="U47" t="n">
         <v>2192471984</v>
       </c>
-      <c r="U47" t="n">
+      <c r="V47" t="n">
         <v>2143773746</v>
       </c>
-      <c r="V47" t="n">
+      <c r="W47" t="n">
         <v>4336247546</v>
       </c>
     </row>
@@ -3808,30 +3951,33 @@
         <v>39.2617960838174</v>
       </c>
       <c r="N48" t="n">
+        <v>3090361014</v>
+      </c>
+      <c r="O48" t="n">
         <v>222107021</v>
       </c>
-      <c r="O48" t="n">
+      <c r="P48" t="n">
         <v>280057565</v>
       </c>
-      <c r="P48" t="n">
+      <c r="Q48" t="n">
         <v>502160379</v>
       </c>
-      <c r="Q48" t="n">
+      <c r="R48" t="n">
         <v>957118860</v>
       </c>
-      <c r="R48" t="n">
+      <c r="S48" t="n">
         <v>894101647</v>
       </c>
-      <c r="S48" t="n">
+      <c r="T48" t="n">
         <v>1851225924</v>
       </c>
-      <c r="T48" t="n">
+      <c r="U48" t="n">
         <v>2225660891</v>
       </c>
-      <c r="U48" t="n">
+      <c r="V48" t="n">
         <v>2175412341</v>
       </c>
-      <c r="V48" t="n">
+      <c r="W48" t="n">
         <v>4401072020</v>
       </c>
     </row>
@@ -3878,30 +4024,33 @@
         <v>39.22134866570068</v>
       </c>
       <c r="N49" t="n">
+        <v>3123387038</v>
+      </c>
+      <c r="O49" t="n">
         <v>226798888</v>
       </c>
-      <c r="O49" t="n">
+      <c r="P49" t="n">
         <v>285514656</v>
       </c>
-      <c r="P49" t="n">
+      <c r="Q49" t="n">
         <v>512310767</v>
       </c>
-      <c r="Q49" t="n">
+      <c r="R49" t="n">
         <v>961941811</v>
       </c>
-      <c r="R49" t="n">
+      <c r="S49" t="n">
         <v>898428955</v>
       </c>
-      <c r="S49" t="n">
+      <c r="T49" t="n">
         <v>1860376010</v>
       </c>
-      <c r="T49" t="n">
+      <c r="U49" t="n">
         <v>2258177862</v>
       </c>
-      <c r="U49" t="n">
+      <c r="V49" t="n">
         <v>2206281587</v>
       </c>
-      <c r="V49" t="n">
+      <c r="W49" t="n">
         <v>4464456992</v>
       </c>
     </row>
@@ -3948,30 +4097,33 @@
         <v>39.10182451866498</v>
       </c>
       <c r="N50" t="n">
+        <v>3152655443</v>
+      </c>
+      <c r="O50" t="n">
         <v>231918472</v>
       </c>
-      <c r="O50" t="n">
+      <c r="P50" t="n">
         <v>291676040</v>
       </c>
-      <c r="P50" t="n">
+      <c r="Q50" t="n">
         <v>523594518</v>
       </c>
-      <c r="Q50" t="n">
+      <c r="R50" t="n">
         <v>966669617</v>
       </c>
-      <c r="R50" t="n">
+      <c r="S50" t="n">
         <v>902703156</v>
       </c>
-      <c r="S50" t="n">
+      <c r="T50" t="n">
         <v>1869372815</v>
       </c>
-      <c r="T50" t="n">
+      <c r="U50" t="n">
         <v>2290075212</v>
       </c>
-      <c r="U50" t="n">
+      <c r="V50" t="n">
         <v>2236434970</v>
       </c>
-      <c r="V50" t="n">
+      <c r="W50" t="n">
         <v>4526510133</v>
       </c>
     </row>
@@ -4018,30 +4170,33 @@
         <v>38.99826590760524</v>
       </c>
       <c r="N51" t="n">
+        <v>3183946265</v>
+      </c>
+      <c r="O51" t="n">
         <v>238213477</v>
       </c>
-      <c r="O51" t="n">
+      <c r="P51" t="n">
         <v>298568959</v>
       </c>
-      <c r="P51" t="n">
+      <c r="Q51" t="n">
         <v>536777826</v>
       </c>
-      <c r="Q51" t="n">
+      <c r="R51" t="n">
         <v>972251569</v>
       </c>
-      <c r="R51" t="n">
+      <c r="S51" t="n">
         <v>908010567</v>
       </c>
-      <c r="S51" t="n">
+      <c r="T51" t="n">
         <v>1880268991</v>
       </c>
-      <c r="T51" t="n">
+      <c r="U51" t="n">
         <v>2319165198</v>
       </c>
-      <c r="U51" t="n">
+      <c r="V51" t="n">
         <v>2264296046</v>
       </c>
-      <c r="V51" t="n">
+      <c r="W51" t="n">
         <v>4583458995</v>
       </c>
     </row>
@@ -4088,30 +4243,33 @@
         <v>38.90701890801686</v>
       </c>
       <c r="N52" t="n">
+        <v>3218194184</v>
+      </c>
+      <c r="O52" t="n">
         <v>244914071</v>
       </c>
-      <c r="O52" t="n">
+      <c r="P52" t="n">
         <v>306233426</v>
       </c>
-      <c r="P52" t="n">
+      <c r="Q52" t="n">
         <v>551140642</v>
       </c>
-      <c r="Q52" t="n">
+      <c r="R52" t="n">
         <v>977693169</v>
       </c>
-      <c r="R52" t="n">
+      <c r="S52" t="n">
         <v>913219073</v>
       </c>
-      <c r="S52" t="n">
+      <c r="T52" t="n">
         <v>1890920283</v>
       </c>
-      <c r="T52" t="n">
+      <c r="U52" t="n">
         <v>2348801393</v>
       </c>
-      <c r="U52" t="n">
+      <c r="V52" t="n">
         <v>2292589146</v>
       </c>
-      <c r="V52" t="n">
+      <c r="W52" t="n">
         <v>4641389354</v>
       </c>
     </row>
@@ -4158,30 +4316,33 @@
         <v>38.88186783576047</v>
       </c>
       <c r="N53" t="n">
+        <v>3250599724</v>
+      </c>
+      <c r="O53" t="n">
         <v>252106319</v>
       </c>
-      <c r="O53" t="n">
+      <c r="P53" t="n">
         <v>314699076</v>
       </c>
-      <c r="P53" t="n">
+      <c r="Q53" t="n">
         <v>566798712</v>
       </c>
-      <c r="Q53" t="n">
+      <c r="R53" t="n">
         <v>983081263</v>
       </c>
-      <c r="R53" t="n">
+      <c r="S53" t="n">
         <v>918423603</v>
       </c>
-      <c r="S53" t="n">
+      <c r="T53" t="n">
         <v>1901511105</v>
       </c>
-      <c r="T53" t="n">
+      <c r="U53" t="n">
         <v>2378401538</v>
       </c>
-      <c r="U53" t="n">
+      <c r="V53" t="n">
         <v>2320663107</v>
       </c>
-      <c r="V53" t="n">
+      <c r="W53" t="n">
         <v>4699065073</v>
       </c>
     </row>
@@ -4228,30 +4389,33 @@
         <v>38.86416104658078</v>
       </c>
       <c r="N54" t="n">
+        <v>3283330912</v>
+      </c>
+      <c r="O54" t="n">
         <v>260008753</v>
       </c>
-      <c r="O54" t="n">
+      <c r="P54" t="n">
         <v>324104379</v>
       </c>
-      <c r="P54" t="n">
+      <c r="Q54" t="n">
         <v>584108969</v>
       </c>
-      <c r="Q54" t="n">
+      <c r="R54" t="n">
         <v>988580820</v>
       </c>
-      <c r="R54" t="n">
+      <c r="S54" t="n">
         <v>923800942</v>
       </c>
-      <c r="S54" t="n">
+      <c r="T54" t="n">
         <v>1912385201</v>
       </c>
-      <c r="T54" t="n">
+      <c r="U54" t="n">
         <v>2407546691</v>
       </c>
-      <c r="U54" t="n">
+      <c r="V54" t="n">
         <v>2347987943</v>
       </c>
-      <c r="V54" t="n">
+      <c r="W54" t="n">
         <v>4755535355</v>
       </c>
     </row>
@@ -4298,30 +4462,33 @@
         <v>38.87177636307433</v>
       </c>
       <c r="N55" t="n">
+        <v>3319710285</v>
+      </c>
+      <c r="O55" t="n">
         <v>268746349</v>
       </c>
-      <c r="O55" t="n">
+      <c r="P55" t="n">
         <v>334532624</v>
       </c>
-      <c r="P55" t="n">
+      <c r="Q55" t="n">
         <v>603278969</v>
       </c>
-      <c r="Q55" t="n">
+      <c r="R55" t="n">
         <v>994159413</v>
       </c>
-      <c r="R55" t="n">
+      <c r="S55" t="n">
         <v>929317279</v>
       </c>
-      <c r="S55" t="n">
+      <c r="T55" t="n">
         <v>1923476702</v>
       </c>
-      <c r="T55" t="n">
+      <c r="U55" t="n">
         <v>2435915269</v>
       </c>
-      <c r="U55" t="n">
+      <c r="V55" t="n">
         <v>2374183731</v>
       </c>
-      <c r="V55" t="n">
+      <c r="W55" t="n">
         <v>4810098991</v>
       </c>
     </row>
@@ -4368,30 +4535,33 @@
         <v>38.88328187213113</v>
       </c>
       <c r="N56" t="n">
+        <v>3354403108</v>
+      </c>
+      <c r="O56" t="n">
         <v>279268134</v>
       </c>
-      <c r="O56" t="n">
+      <c r="P56" t="n">
         <v>346160757</v>
       </c>
-      <c r="P56" t="n">
+      <c r="Q56" t="n">
         <v>625426009</v>
       </c>
-      <c r="Q56" t="n">
+      <c r="R56" t="n">
         <v>1000025001</v>
       </c>
-      <c r="R56" t="n">
+      <c r="S56" t="n">
         <v>935328390</v>
       </c>
-      <c r="S56" t="n">
+      <c r="T56" t="n">
         <v>1935358125</v>
       </c>
-      <c r="T56" t="n">
+      <c r="U56" t="n">
         <v>2462572821</v>
       </c>
-      <c r="U56" t="n">
+      <c r="V56" t="n">
         <v>2398890779</v>
       </c>
-      <c r="V56" t="n">
+      <c r="W56" t="n">
         <v>4861461723</v>
       </c>
     </row>
@@ -4438,30 +4608,33 @@
         <v>38.89739184677391</v>
       </c>
       <c r="N57" t="n">
+        <v>3391647862</v>
+      </c>
+      <c r="O57" t="n">
         <v>290411331</v>
       </c>
-      <c r="O57" t="n">
+      <c r="P57" t="n">
         <v>358609161</v>
       </c>
-      <c r="P57" t="n">
+      <c r="Q57" t="n">
         <v>649016774</v>
       </c>
-      <c r="Q57" t="n">
+      <c r="R57" t="n">
         <v>1005787566</v>
       </c>
-      <c r="R57" t="n">
+      <c r="S57" t="n">
         <v>941262629</v>
       </c>
-      <c r="S57" t="n">
+      <c r="T57" t="n">
         <v>1947058373</v>
       </c>
-      <c r="T57" t="n">
+      <c r="U57" t="n">
         <v>2488493425</v>
       </c>
-      <c r="U57" t="n">
+      <c r="V57" t="n">
         <v>2422523214</v>
       </c>
-      <c r="V57" t="n">
+      <c r="W57" t="n">
         <v>4911012178</v>
       </c>
     </row>
@@ -4508,30 +4681,33 @@
         <v>38.91647162843554</v>
       </c>
       <c r="N58" t="n">
+        <v>3427481440</v>
+      </c>
+      <c r="O58" t="n">
         <v>301860619</v>
       </c>
-      <c r="O58" t="n">
+      <c r="P58" t="n">
         <v>371579629</v>
       </c>
-      <c r="P58" t="n">
+      <c r="Q58" t="n">
         <v>673436939</v>
       </c>
-      <c r="Q58" t="n">
+      <c r="R58" t="n">
         <v>1011137062</v>
       </c>
-      <c r="R58" t="n">
+      <c r="S58" t="n">
         <v>946850097</v>
       </c>
-      <c r="S58" t="n">
+      <c r="T58" t="n">
         <v>1957996874</v>
       </c>
-      <c r="T58" t="n">
+      <c r="U58" t="n">
         <v>2513570542</v>
       </c>
-      <c r="U58" t="n">
+      <c r="V58" t="n">
         <v>2445023359</v>
       </c>
-      <c r="V58" t="n">
+      <c r="W58" t="n">
         <v>4958587504</v>
       </c>
     </row>
@@ -4578,30 +4754,33 @@
         <v>43.5523287209535</v>
       </c>
       <c r="N59" t="n">
+        <v>199217046</v>
+      </c>
+      <c r="O59" t="n">
         <v>26983341</v>
       </c>
-      <c r="O59" t="n">
+      <c r="P59" t="n">
         <v>40416964</v>
       </c>
-      <c r="P59" t="n">
+      <c r="Q59" t="n">
         <v>67400323</v>
       </c>
-      <c r="Q59" t="n">
+      <c r="R59" t="n">
         <v>37177191</v>
       </c>
-      <c r="R59" t="n">
+      <c r="S59" t="n">
         <v>35331567</v>
       </c>
-      <c r="S59" t="n">
+      <c r="T59" t="n">
         <v>72508771</v>
       </c>
-      <c r="T59" t="n">
+      <c r="U59" t="n">
         <v>144851384</v>
       </c>
-      <c r="U59" t="n">
+      <c r="V59" t="n">
         <v>144568168</v>
       </c>
-      <c r="V59" t="n">
+      <c r="W59" t="n">
         <v>289419527</v>
       </c>
     </row>
@@ -4648,30 +4827,33 @@
         <v>43.64378281174579</v>
       </c>
       <c r="N60" t="n">
+        <v>199487250</v>
+      </c>
+      <c r="O60" t="n">
         <v>27574609</v>
       </c>
-      <c r="O60" t="n">
+      <c r="P60" t="n">
         <v>40935135</v>
       </c>
-      <c r="P60" t="n">
+      <c r="Q60" t="n">
         <v>68508730</v>
       </c>
-      <c r="Q60" t="n">
+      <c r="R60" t="n">
         <v>36683582</v>
       </c>
-      <c r="R60" t="n">
+      <c r="S60" t="n">
         <v>34867727</v>
       </c>
-      <c r="S60" t="n">
+      <c r="T60" t="n">
         <v>71551630</v>
       </c>
-      <c r="T60" t="n">
+      <c r="U60" t="n">
         <v>145066056</v>
       </c>
-      <c r="U60" t="n">
+      <c r="V60" t="n">
         <v>144768523</v>
       </c>
-      <c r="V60" t="n">
+      <c r="W60" t="n">
         <v>289835272</v>
       </c>
     </row>
@@ -4718,30 +4900,33 @@
         <v>43.78733537480365</v>
       </c>
       <c r="N61" t="n">
+        <v>200144636</v>
+      </c>
+      <c r="O61" t="n">
         <v>28190807</v>
       </c>
-      <c r="O61" t="n">
+      <c r="P61" t="n">
         <v>41510324</v>
       </c>
-      <c r="P61" t="n">
+      <c r="Q61" t="n">
         <v>69700019</v>
       </c>
-      <c r="Q61" t="n">
+      <c r="R61" t="n">
         <v>36239064</v>
       </c>
-      <c r="R61" t="n">
+      <c r="S61" t="n">
         <v>34445583</v>
       </c>
-      <c r="S61" t="n">
+      <c r="T61" t="n">
         <v>70685008</v>
       </c>
-      <c r="T61" t="n">
+      <c r="U61" t="n">
         <v>145423802</v>
       </c>
-      <c r="U61" t="n">
+      <c r="V61" t="n">
         <v>145072358</v>
       </c>
-      <c r="V61" t="n">
+      <c r="W61" t="n">
         <v>290496921</v>
       </c>
     </row>
@@ -4788,30 +4973,33 @@
         <v>43.99929887773144</v>
       </c>
       <c r="N62" t="n">
+        <v>201933394</v>
+      </c>
+      <c r="O62" t="n">
         <v>28822235</v>
       </c>
-      <c r="O62" t="n">
+      <c r="P62" t="n">
         <v>42133057</v>
       </c>
-      <c r="P62" t="n">
+      <c r="Q62" t="n">
         <v>70954595</v>
       </c>
-      <c r="Q62" t="n">
+      <c r="R62" t="n">
         <v>35865768</v>
       </c>
-      <c r="R62" t="n">
+      <c r="S62" t="n">
         <v>34089653</v>
       </c>
-      <c r="S62" t="n">
+      <c r="T62" t="n">
         <v>69955653</v>
       </c>
-      <c r="T62" t="n">
+      <c r="U62" t="n">
         <v>145967633</v>
       </c>
-      <c r="U62" t="n">
+      <c r="V62" t="n">
         <v>145537594</v>
       </c>
-      <c r="V62" t="n">
+      <c r="W62" t="n">
         <v>291505694</v>
       </c>
     </row>
@@ -4858,30 +5046,33 @@
         <v>44.13903932683652</v>
       </c>
       <c r="N63" t="n">
+        <v>203395227</v>
+      </c>
+      <c r="O63" t="n">
         <v>29404371</v>
       </c>
-      <c r="O63" t="n">
+      <c r="P63" t="n">
         <v>42723982</v>
       </c>
-      <c r="P63" t="n">
+      <c r="Q63" t="n">
         <v>72128136</v>
       </c>
-      <c r="Q63" t="n">
+      <c r="R63" t="n">
         <v>35545528</v>
       </c>
-      <c r="R63" t="n">
+      <c r="S63" t="n">
         <v>33785243</v>
       </c>
-      <c r="S63" t="n">
+      <c r="T63" t="n">
         <v>69330853</v>
       </c>
-      <c r="T63" t="n">
+      <c r="U63" t="n">
         <v>146546226</v>
       </c>
-      <c r="U63" t="n">
+      <c r="V63" t="n">
         <v>146034888</v>
       </c>
-      <c r="V63" t="n">
+      <c r="W63" t="n">
         <v>292581249</v>
       </c>
     </row>
@@ -4928,30 +5119,33 @@
         <v>44.2474092696829</v>
       </c>
       <c r="N64" t="n">
+        <v>205365646</v>
+      </c>
+      <c r="O64" t="n">
         <v>29908385</v>
       </c>
-      <c r="O64" t="n">
+      <c r="P64" t="n">
         <v>43248039</v>
       </c>
-      <c r="P64" t="n">
+      <c r="Q64" t="n">
         <v>73156433</v>
       </c>
-      <c r="Q64" t="n">
+      <c r="R64" t="n">
         <v>35275100</v>
       </c>
-      <c r="R64" t="n">
+      <c r="S64" t="n">
         <v>33529537</v>
       </c>
-      <c r="S64" t="n">
+      <c r="T64" t="n">
         <v>68804626</v>
       </c>
-      <c r="T64" t="n">
+      <c r="U64" t="n">
         <v>147100873</v>
       </c>
-      <c r="U64" t="n">
+      <c r="V64" t="n">
         <v>146520012</v>
       </c>
-      <c r="V64" t="n">
+      <c r="W64" t="n">
         <v>293620893</v>
       </c>
     </row>
@@ -4998,30 +5192,33 @@
         <v>44.45184477308837</v>
       </c>
       <c r="N65" t="n">
+        <v>206996811</v>
+      </c>
+      <c r="O65" t="n">
         <v>30480380</v>
       </c>
-      <c r="O65" t="n">
+      <c r="P65" t="n">
         <v>43743438</v>
       </c>
-      <c r="P65" t="n">
+      <c r="Q65" t="n">
         <v>74223643</v>
       </c>
-      <c r="Q65" t="n">
+      <c r="R65" t="n">
         <v>35150050</v>
       </c>
-      <c r="R65" t="n">
+      <c r="S65" t="n">
         <v>33395964</v>
       </c>
-      <c r="S65" t="n">
+      <c r="T65" t="n">
         <v>68546087</v>
       </c>
-      <c r="T65" t="n">
+      <c r="U65" t="n">
         <v>147366627</v>
       </c>
-      <c r="U65" t="n">
+      <c r="V65" t="n">
         <v>146861590</v>
       </c>
-      <c r="V65" t="n">
+      <c r="W65" t="n">
         <v>294228323</v>
       </c>
     </row>
@@ -5068,30 +5265,33 @@
         <v>44.57560018196742</v>
       </c>
       <c r="N66" t="n">
+        <v>208540629</v>
+      </c>
+      <c r="O66" t="n">
         <v>30977641</v>
       </c>
-      <c r="O66" t="n">
+      <c r="P66" t="n">
         <v>44167962</v>
       </c>
-      <c r="P66" t="n">
+      <c r="Q66" t="n">
         <v>75144939</v>
       </c>
-      <c r="Q66" t="n">
+      <c r="R66" t="n">
         <v>35079113</v>
       </c>
-      <c r="R66" t="n">
+      <c r="S66" t="n">
         <v>33319358</v>
       </c>
-      <c r="S66" t="n">
+      <c r="T66" t="n">
         <v>68398708</v>
       </c>
-      <c r="T66" t="n">
+      <c r="U66" t="n">
         <v>147668376</v>
       </c>
-      <c r="U66" t="n">
+      <c r="V66" t="n">
         <v>147255954</v>
       </c>
-      <c r="V66" t="n">
+      <c r="W66" t="n">
         <v>294924755</v>
       </c>
     </row>
@@ -5138,30 +5338,33 @@
         <v>44.72240568076412</v>
       </c>
       <c r="N67" t="n">
+        <v>210215521</v>
+      </c>
+      <c r="O67" t="n">
         <v>31440947</v>
       </c>
-      <c r="O67" t="n">
+      <c r="P67" t="n">
         <v>44565794</v>
       </c>
-      <c r="P67" t="n">
+      <c r="Q67" t="n">
         <v>76005592</v>
       </c>
-      <c r="Q67" t="n">
+      <c r="R67" t="n">
         <v>35040329</v>
       </c>
-      <c r="R67" t="n">
+      <c r="S67" t="n">
         <v>33278780</v>
       </c>
-      <c r="S67" t="n">
+      <c r="T67" t="n">
         <v>68319523</v>
       </c>
-      <c r="T67" t="n">
+      <c r="U67" t="n">
         <v>147934404</v>
       </c>
-      <c r="U67" t="n">
+      <c r="V67" t="n">
         <v>147616420</v>
       </c>
-      <c r="V67" t="n">
+      <c r="W67" t="n">
         <v>295551560</v>
       </c>
     </row>
@@ -5208,30 +5411,33 @@
         <v>44.97392184015619</v>
       </c>
       <c r="N68" t="n">
+        <v>210743587</v>
+      </c>
+      <c r="O68" t="n">
         <v>31918126</v>
       </c>
-      <c r="O68" t="n">
+      <c r="P68" t="n">
         <v>44992413</v>
       </c>
-      <c r="P68" t="n">
+      <c r="Q68" t="n">
         <v>76909417</v>
       </c>
-      <c r="Q68" t="n">
+      <c r="R68" t="n">
         <v>34982826</v>
       </c>
-      <c r="R68" t="n">
+      <c r="S68" t="n">
         <v>33222483</v>
       </c>
-      <c r="S68" t="n">
+      <c r="T68" t="n">
         <v>68205703</v>
       </c>
-      <c r="T68" t="n">
+      <c r="U68" t="n">
         <v>148025937</v>
       </c>
-      <c r="U68" t="n">
+      <c r="V68" t="n">
         <v>147776012</v>
       </c>
-      <c r="V68" t="n">
+      <c r="W68" t="n">
         <v>295802677</v>
       </c>
     </row>
@@ -5278,30 +5484,33 @@
         <v>45.14588478545598</v>
       </c>
       <c r="N69" t="n">
+        <v>211354253</v>
+      </c>
+      <c r="O69" t="n">
         <v>32456153</v>
       </c>
-      <c r="O69" t="n">
+      <c r="P69" t="n">
         <v>45507432</v>
       </c>
-      <c r="P69" t="n">
+      <c r="Q69" t="n">
         <v>77963571</v>
       </c>
-      <c r="Q69" t="n">
+      <c r="R69" t="n">
         <v>34882066</v>
       </c>
-      <c r="R69" t="n">
+      <c r="S69" t="n">
         <v>33121786</v>
       </c>
-      <c r="S69" t="n">
+      <c r="T69" t="n">
         <v>68003865</v>
       </c>
-      <c r="T69" t="n">
+      <c r="U69" t="n">
         <v>147900423</v>
       </c>
-      <c r="U69" t="n">
+      <c r="V69" t="n">
         <v>147664549</v>
       </c>
-      <c r="V69" t="n">
+      <c r="W69" t="n">
         <v>295564975</v>
       </c>
     </row>
@@ -5348,30 +5557,33 @@
         <v>45.3379288813376</v>
       </c>
       <c r="N70" t="n">
+        <v>210739030</v>
+      </c>
+      <c r="O70" t="n">
         <v>33001840</v>
       </c>
-      <c r="O70" t="n">
+      <c r="P70" t="n">
         <v>45918187</v>
       </c>
-      <c r="P70" t="n">
+      <c r="Q70" t="n">
         <v>78917515</v>
       </c>
-      <c r="Q70" t="n">
+      <c r="R70" t="n">
         <v>34828360</v>
       </c>
-      <c r="R70" t="n">
+      <c r="S70" t="n">
         <v>33057673</v>
       </c>
-      <c r="S70" t="n">
+      <c r="T70" t="n">
         <v>67886842</v>
       </c>
-      <c r="T70" t="n">
+      <c r="U70" t="n">
         <v>147041562</v>
       </c>
-      <c r="U70" t="n">
+      <c r="V70" t="n">
         <v>146899361</v>
       </c>
-      <c r="V70" t="n">
+      <c r="W70" t="n">
         <v>293942620</v>
       </c>
     </row>
@@ -5418,30 +5630,33 @@
         <v>45.51158241410484</v>
       </c>
       <c r="N71" t="n">
+        <v>212039861</v>
+      </c>
+      <c r="O71" t="n">
         <v>33755536</v>
       </c>
-      <c r="O71" t="n">
+      <c r="P71" t="n">
         <v>46622329</v>
       </c>
-      <c r="P71" t="n">
+      <c r="Q71" t="n">
         <v>80374178</v>
       </c>
-      <c r="Q71" t="n">
+      <c r="R71" t="n">
         <v>34793521</v>
       </c>
-      <c r="R71" t="n">
+      <c r="S71" t="n">
         <v>33010219</v>
       </c>
-      <c r="S71" t="n">
+      <c r="T71" t="n">
         <v>67804934</v>
       </c>
-      <c r="T71" t="n">
+      <c r="U71" t="n">
         <v>146664700</v>
       </c>
-      <c r="U71" t="n">
+      <c r="V71" t="n">
         <v>146549627</v>
       </c>
-      <c r="V71" t="n">
+      <c r="W71" t="n">
         <v>293216813</v>
       </c>
     </row>
@@ -5488,30 +5703,33 @@
         <v>45.65044273429207</v>
       </c>
       <c r="N72" t="n">
+        <v>212597037</v>
+      </c>
+      <c r="O72" t="n">
         <v>34601585</v>
       </c>
-      <c r="O72" t="n">
+      <c r="P72" t="n">
         <v>47480483</v>
       </c>
-      <c r="P72" t="n">
+      <c r="Q72" t="n">
         <v>82078616</v>
       </c>
-      <c r="Q72" t="n">
+      <c r="R72" t="n">
         <v>34749885</v>
       </c>
-      <c r="R72" t="n">
+      <c r="S72" t="n">
         <v>32952136</v>
       </c>
-      <c r="S72" t="n">
+      <c r="T72" t="n">
         <v>67703125</v>
       </c>
-      <c r="T72" t="n">
+      <c r="U72" t="n">
         <v>146418095</v>
       </c>
-      <c r="U72" t="n">
+      <c r="V72" t="n">
         <v>146267291</v>
       </c>
-      <c r="V72" t="n">
+      <c r="W72" t="n">
         <v>292687731</v>
       </c>
     </row>
@@ -5558,30 +5776,33 @@
         <v>45.72787895218688</v>
       </c>
       <c r="N73" t="n">
+        <v>213265285</v>
+      </c>
+      <c r="O73" t="n">
         <v>35454260</v>
       </c>
-      <c r="O73" t="n">
+      <c r="P73" t="n">
         <v>48384702</v>
       </c>
-      <c r="P73" t="n">
+      <c r="Q73" t="n">
         <v>83836853</v>
       </c>
-      <c r="Q73" t="n">
+      <c r="R73" t="n">
         <v>34726527</v>
       </c>
-      <c r="R73" t="n">
+      <c r="S73" t="n">
         <v>32911492</v>
       </c>
-      <c r="S73" t="n">
+      <c r="T73" t="n">
         <v>67638708</v>
       </c>
-      <c r="T73" t="n">
+      <c r="U73" t="n">
         <v>146175382</v>
       </c>
-      <c r="U73" t="n">
+      <c r="V73" t="n">
         <v>145924299</v>
       </c>
-      <c r="V73" t="n">
+      <c r="W73" t="n">
         <v>292101100</v>
       </c>
     </row>
@@ -5628,30 +5849,33 @@
         <v>45.74019096896031</v>
       </c>
       <c r="N74" t="n">
+        <v>213640167</v>
+      </c>
+      <c r="O74" t="n">
         <v>36267554</v>
       </c>
-      <c r="O74" t="n">
+      <c r="P74" t="n">
         <v>49271108</v>
       </c>
-      <c r="P74" t="n">
+      <c r="Q74" t="n">
         <v>85538662</v>
       </c>
-      <c r="Q74" t="n">
+      <c r="R74" t="n">
         <v>34736210</v>
       </c>
-      <c r="R74" t="n">
+      <c r="S74" t="n">
         <v>32900347</v>
       </c>
-      <c r="S74" t="n">
+      <c r="T74" t="n">
         <v>67636573</v>
       </c>
-      <c r="T74" t="n">
+      <c r="U74" t="n">
         <v>145889436</v>
       </c>
-      <c r="U74" t="n">
+      <c r="V74" t="n">
         <v>145479100</v>
       </c>
-      <c r="V74" t="n">
+      <c r="W74" t="n">
         <v>291368526</v>
       </c>
     </row>
@@ -5698,30 +5922,33 @@
         <v>45.80899885365794</v>
       </c>
       <c r="N75" t="n">
+        <v>214618312</v>
+      </c>
+      <c r="O75" t="n">
         <v>37089281</v>
       </c>
-      <c r="O75" t="n">
+      <c r="P75" t="n">
         <v>50063869</v>
       </c>
-      <c r="P75" t="n">
+      <c r="Q75" t="n">
         <v>87152447</v>
       </c>
-      <c r="Q75" t="n">
+      <c r="R75" t="n">
         <v>34691936</v>
       </c>
-      <c r="R75" t="n">
+      <c r="S75" t="n">
         <v>32849579</v>
       </c>
-      <c r="S75" t="n">
+      <c r="T75" t="n">
         <v>67541776</v>
       </c>
-      <c r="T75" t="n">
+      <c r="U75" t="n">
         <v>145654074</v>
       </c>
-      <c r="U75" t="n">
+      <c r="V75" t="n">
         <v>145136345</v>
       </c>
-      <c r="V75" t="n">
+      <c r="W75" t="n">
         <v>290790854</v>
       </c>
     </row>
@@ -5768,30 +5995,33 @@
         <v>45.83351665611057</v>
       </c>
       <c r="N76" t="n">
+        <v>215671511</v>
+      </c>
+      <c r="O76" t="n">
         <v>37838290</v>
       </c>
-      <c r="O76" t="n">
+      <c r="P76" t="n">
         <v>50801131</v>
       </c>
-      <c r="P76" t="n">
+      <c r="Q76" t="n">
         <v>88638593</v>
       </c>
-      <c r="Q76" t="n">
+      <c r="R76" t="n">
         <v>34714260</v>
       </c>
-      <c r="R76" t="n">
+      <c r="S76" t="n">
         <v>32858413</v>
       </c>
-      <c r="S76" t="n">
+      <c r="T76" t="n">
         <v>67573005</v>
       </c>
-      <c r="T76" t="n">
+      <c r="U76" t="n">
         <v>145294518</v>
       </c>
-      <c r="U76" t="n">
+      <c r="V76" t="n">
         <v>144625627</v>
       </c>
-      <c r="V76" t="n">
+      <c r="W76" t="n">
         <v>289920642</v>
       </c>
     </row>
@@ -5838,30 +6068,33 @@
         <v>45.84576157509888</v>
       </c>
       <c r="N77" t="n">
+        <v>216488451</v>
+      </c>
+      <c r="O77" t="n">
         <v>38556689</v>
       </c>
-      <c r="O77" t="n">
+      <c r="P77" t="n">
         <v>51530044</v>
       </c>
-      <c r="P77" t="n">
+      <c r="Q77" t="n">
         <v>90085964</v>
       </c>
-      <c r="Q77" t="n">
+      <c r="R77" t="n">
         <v>34775123</v>
       </c>
-      <c r="R77" t="n">
+      <c r="S77" t="n">
         <v>32903910</v>
       </c>
-      <c r="S77" t="n">
+      <c r="T77" t="n">
         <v>67679351</v>
       </c>
-      <c r="T77" t="n">
+      <c r="U77" t="n">
         <v>144936889</v>
       </c>
-      <c r="U77" t="n">
+      <c r="V77" t="n">
         <v>144083636</v>
       </c>
-      <c r="V77" t="n">
+      <c r="W77" t="n">
         <v>289020974</v>
       </c>
     </row>

</xml_diff>